<commit_message>
minor example file changes
</commit_message>
<xml_diff>
--- a/cgmanalysis/inst/extdata/De-identified/iPro.xlsx
+++ b/cgmanalysis/inst/extdata/De-identified/iPro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timbv\Documents\GitHub\R-Packages\cgmanalysis\inst\extdata\De-identified\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566E415C-E145-447C-8C62-EFBCFD8F8A6B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF13E2B2-7679-4FBF-9085-30CF8E34C1F8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1023,7 +1023,7 @@
   <dimension ref="A1:V2063"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>